<commit_message>
Task Sheet updated 07/03/2019
</commit_message>
<xml_diff>
--- a/Task.xlsx
+++ b/Task.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="630" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="overAllChart" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="98">
   <si>
     <t>customer</t>
   </si>
@@ -110,12 +110,6 @@
     <t>InventoryDetails</t>
   </si>
   <si>
-    <t>InventoryLogin</t>
-  </si>
-  <si>
-    <t>InventoryRegister</t>
-  </si>
-  <si>
     <t>utility</t>
   </si>
   <si>
@@ -170,18 +164,6 @@
     <t>InventoryCatalog</t>
   </si>
   <si>
-    <t>InventoryLaptop</t>
-  </si>
-  <si>
-    <t>InventoryDesktop</t>
-  </si>
-  <si>
-    <t>InventoryTablet</t>
-  </si>
-  <si>
-    <t>InventoryServer</t>
-  </si>
-  <si>
     <t>InventoryReport</t>
   </si>
   <si>
@@ -306,6 +288,33 @@
   </si>
   <si>
     <t>tables and columns are created and updated in github</t>
+  </si>
+  <si>
+    <t>InventoryDdsClient</t>
+  </si>
+  <si>
+    <t>InventoryDdsClientInfo</t>
+  </si>
+  <si>
+    <t>InventoryRunningCustomer</t>
+  </si>
+  <si>
+    <t>InventoryRunningCustomerInfo</t>
+  </si>
+  <si>
+    <t>InventoryReseller</t>
+  </si>
+  <si>
+    <t>InventoryResellerInfo</t>
+  </si>
+  <si>
+    <t>InventoryManuallyInsertingModule</t>
+  </si>
+  <si>
+    <t>InventoryRunningCustomerReport</t>
+  </si>
+  <si>
+    <t>InventoryResellerReport</t>
   </si>
 </sst>
 </file>
@@ -673,8 +682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G6" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,7 +709,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -709,10 +718,10 @@
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -724,7 +733,7 @@
         <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -735,7 +744,7 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -752,7 +761,7 @@
         <v>43648</v>
       </c>
       <c r="F4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="H4" t="s">
         <v>15</v>
@@ -777,7 +786,7 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -785,7 +794,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -809,13 +818,13 @@
         <v>43801</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="H13" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="I13" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="J13" t="s">
         <v>16</v>
@@ -826,7 +835,7 @@
         <v>20</v>
       </c>
       <c r="E14" s="7">
-        <v>43468</v>
+        <v>43649</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -846,10 +855,10 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B21" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D21" s="3">
         <v>43679</v>
@@ -858,7 +867,7 @@
         <v>43771</v>
       </c>
       <c r="F21" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="H21" t="s">
         <v>15</v>
@@ -872,23 +881,29 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>70</v>
+        <v>64</v>
+      </c>
+      <c r="D22" s="3">
+        <v>43558</v>
+      </c>
+      <c r="E22" s="3">
+        <v>43591</v>
       </c>
       <c r="F22" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F24" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -902,10 +917,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -940,7 +955,7 @@
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -961,171 +976,216 @@
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G4" t="s">
-        <v>29</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G5" t="s">
-        <v>30</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G7" t="s">
-        <v>33</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G8" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
-        <v>35</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G10" t="s">
-        <v>36</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G11" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G12" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G13" t="s">
-        <v>39</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G14" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G15" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G16" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G17" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G18" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G19" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G20" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G21" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G22" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G23" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G24" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G25" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G26" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G27" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G28" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G29" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G30" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G31" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G32" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G33" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
     </row>
     <row r="34" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G34" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G35" t="s">
-        <v>61</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G36" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G37" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G38" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G39" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G40" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G41" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G42" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="43" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G43" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="44" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G44" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1138,10 +1198,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="G5" sqref="G5:G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1155,381 +1215,480 @@
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
       <c r="E1" s="5" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C5" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="G5" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C6" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G6" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>89</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>89</v>
       </c>
       <c r="G8" t="s">
-        <v>33</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="G9" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>91</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>91</v>
       </c>
       <c r="G10" t="s">
-        <v>35</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>92</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>92</v>
       </c>
       <c r="G11" t="s">
-        <v>36</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
       <c r="G12" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="G13" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>95</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>95</v>
       </c>
       <c r="G14" t="s">
-        <v>39</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="G15" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G16" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="G17" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="G18" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="G19" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="G20" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="G21" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C22" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="G22" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C23" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="G23" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="C24" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="G24" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>85</v>
+        <v>41</v>
       </c>
       <c r="C25" t="s">
-        <v>85</v>
+        <v>41</v>
       </c>
       <c r="G25" t="s">
-        <v>85</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>86</v>
+        <v>42</v>
       </c>
       <c r="C26" t="s">
-        <v>86</v>
+        <v>42</v>
       </c>
       <c r="G26" t="s">
-        <v>86</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>87</v>
+        <v>43</v>
       </c>
       <c r="C27" t="s">
-        <v>87</v>
+        <v>43</v>
       </c>
       <c r="G27" t="s">
-        <v>87</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C28" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="G28" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C29" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="G29" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C30" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="G30" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="C31" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="G31" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="C32" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="G32" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="C33" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="G33" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="C34" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="G34" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="C35" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="G35" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C36" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="G36" t="s">
-        <v>61</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>49</v>
+      </c>
+      <c r="C37" t="s">
+        <v>49</v>
+      </c>
+      <c r="G37" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>50</v>
+      </c>
+      <c r="C38" t="s">
+        <v>50</v>
+      </c>
+      <c r="G38" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" t="s">
+        <v>51</v>
+      </c>
+      <c r="G39" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40" t="s">
+        <v>96</v>
+      </c>
+      <c r="G40" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>97</v>
+      </c>
+      <c r="C41" t="s">
+        <v>97</v>
+      </c>
+      <c r="G41" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" t="s">
+        <v>52</v>
+      </c>
+      <c r="G42" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>53</v>
+      </c>
+      <c r="C43" t="s">
+        <v>53</v>
+      </c>
+      <c r="G43" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>54</v>
+      </c>
+      <c r="C44" t="s">
+        <v>54</v>
+      </c>
+      <c r="G44" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" t="s">
+        <v>55</v>
+      </c>
+      <c r="G45" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
11/03/2019 - task sheet updated
</commit_message>
<xml_diff>
--- a/Task.xlsx
+++ b/Task.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="630" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="1260" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="overAllChart" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="99">
   <si>
     <t>customer</t>
   </si>
@@ -315,6 +315,9 @@
   </si>
   <si>
     <t>InventoryResellerReport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">updating methods like existing registered data in db </t>
   </si>
 </sst>
 </file>
@@ -683,7 +686,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,7 +838,10 @@
         <v>20</v>
       </c>
       <c r="E14" s="7">
-        <v>43649</v>
+        <v>43772</v>
+      </c>
+      <c r="F14" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>